<commit_message>
Updated Report Util and Implemented LogOutPage
</commit_message>
<xml_diff>
--- a/src/test/resources/OpenCartTestData.xlsx
+++ b/src/test/resources/OpenCartTestData.xlsx
@@ -3,16 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C2D94ED7-E3E0-4706-8BE9-563530D59205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishnu\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF4C0EC-3674-447C-8790-77F6BDD63CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{6B310937-BDF3-4FAB-93A3-2F5ACE2FEBE1}"/>
+    <workbookView xWindow="4305" yWindow="735" windowWidth="21600" windowHeight="14820" activeTab="1" xr2:uid="{6B310937-BDF3-4FAB-93A3-2F5ACE2FEBE1}"/>
   </bookViews>
   <sheets>
     <sheet name="tests" sheetId="2" r:id="rId1"/>
     <sheet name="data" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="76">
   <si>
     <t>TestCase</t>
   </si>
@@ -75,9 +79,6 @@
     <t>Vishnu123</t>
   </si>
   <si>
-    <t>RegisterTest</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -96,36 +97,18 @@
     <t>ExpectedResult</t>
   </si>
   <si>
-    <t>Abhishek</t>
-  </si>
-  <si>
-    <t>Balraj</t>
-  </si>
-  <si>
     <t>Pawan</t>
   </si>
   <si>
     <t>Abhi</t>
   </si>
   <si>
-    <t>Bal</t>
-  </si>
-  <si>
     <t>Paw</t>
   </si>
   <si>
     <t>autogenerate</t>
   </si>
   <si>
-    <t>Password@123</t>
-  </si>
-  <si>
-    <t>SearchTest</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
     <t>NoCredentilals</t>
   </si>
   <si>
@@ -169,6 +152,108 @@
   </si>
   <si>
     <t>ValidEmail &amp; InvalidPass</t>
+  </si>
+  <si>
+    <t>Trevor</t>
+  </si>
+  <si>
+    <t>Tre</t>
+  </si>
+  <si>
+    <t>PWD Entered ::  All Uppercase</t>
+  </si>
+  <si>
+    <t>PWD Entered ::  All Lowercase</t>
+  </si>
+  <si>
+    <t>PWD Entered ::  All Numbers</t>
+  </si>
+  <si>
+    <t>PWD Entered ::  No Numbers</t>
+  </si>
+  <si>
+    <t>PWD Entered ::  All Special Characters</t>
+  </si>
+  <si>
+    <t>PWD Entered ::  No Special Characters</t>
+  </si>
+  <si>
+    <t>PWD Entered ::  With Spaces</t>
+  </si>
+  <si>
+    <t>password123!</t>
+  </si>
+  <si>
+    <t>PASSWORD123!</t>
+  </si>
+  <si>
+    <t>Password!</t>
+  </si>
+  <si>
+    <t>^$^*^$*^*$</t>
+  </si>
+  <si>
+    <t>Password123</t>
+  </si>
+  <si>
+    <t>Pass word 123!</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Shyam</t>
+  </si>
+  <si>
+    <t>Cohen</t>
+  </si>
+  <si>
+    <t>Lawren</t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>Coh</t>
+  </si>
+  <si>
+    <t>Shy</t>
+  </si>
+  <si>
+    <t>Rah</t>
+  </si>
+  <si>
+    <t>RegisterTest- Password complexity</t>
+  </si>
+  <si>
+    <t>Valid1Password!</t>
+  </si>
+  <si>
+    <t>Phone Text Entered ::  Nine Digits</t>
+  </si>
+  <si>
+    <t>Phone Text Entered :: Non Numeric</t>
+  </si>
+  <si>
+    <t>Phone Text Entered ::  Eleven Digits</t>
+  </si>
+  <si>
+    <t>Phone Text Entered ::   All Special Characters</t>
+  </si>
+  <si>
+    <t>abcdefghij</t>
+  </si>
+  <si>
+    <t>!@#$%^&amp;*()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Phone Text Entered :: With Spaces</t>
+  </si>
+  <si>
+    <t>1234 67 90</t>
+  </si>
+  <si>
+    <t>RegisterTest- InvalidPhone Numbers</t>
   </si>
 </sst>
 </file>
@@ -632,15 +717,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00103B07-0830-4177-83BC-8CB4AFE7543B}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
@@ -648,15 +733,15 @@
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -670,10 +755,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -687,10 +772,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -704,10 +789,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -721,10 +806,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -738,15 +823,15 @@
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
@@ -760,32 +845,32 @@
         <v>10</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>16</v>
@@ -794,10 +879,10 @@
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -805,185 +890,449 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1">
         <v>1234567890</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1">
         <v>1234567890</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E20" s="1">
         <v>1234567890</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>31</v>
+      <c r="F20" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1234567890</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="I20" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="B27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="1">
+        <v>12345678901</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
-        <v>11</v>
+      <c r="C30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -992,15 +1341,26 @@
     <hyperlink ref="B5" r:id="rId2" xr:uid="{EB056E9E-90CA-4EDC-A199-674D1466E349}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{A4C1F655-E25B-4FC6-94CB-4E25C5EFB118}"/>
     <hyperlink ref="B7" r:id="rId4" xr:uid="{4527B624-17F0-40C4-BED7-A03548D332A0}"/>
-    <hyperlink ref="F18" r:id="rId5" xr:uid="{05E54411-6BAE-4BB6-A2ED-14B59F165260}"/>
-    <hyperlink ref="F19" r:id="rId6" xr:uid="{047321AD-B318-46D7-B924-58B664E4DAD4}"/>
-    <hyperlink ref="F20" r:id="rId7" xr:uid="{B0882F14-E495-408B-AE6A-2B6DA9F7C8AD}"/>
-    <hyperlink ref="G18" r:id="rId8" xr:uid="{EF48C1FF-3731-4590-AD35-C77D774E0AB3}"/>
-    <hyperlink ref="G19" r:id="rId9" xr:uid="{D05C35DE-D138-4810-B1AC-59CDB7E5213C}"/>
-    <hyperlink ref="G20" r:id="rId10" xr:uid="{8C9443A3-AC63-4830-AA68-FED07FD75DF1}"/>
+    <hyperlink ref="F18" r:id="rId5" display="Password@123" xr:uid="{05E54411-6BAE-4BB6-A2ED-14B59F165260}"/>
+    <hyperlink ref="F19" r:id="rId6" display="Password@123" xr:uid="{047321AD-B318-46D7-B924-58B664E4DAD4}"/>
+    <hyperlink ref="F20" r:id="rId7" display="Password@123" xr:uid="{B0882F14-E495-408B-AE6A-2B6DA9F7C8AD}"/>
+    <hyperlink ref="G18" r:id="rId8" display="Password@123" xr:uid="{EF48C1FF-3731-4590-AD35-C77D774E0AB3}"/>
+    <hyperlink ref="G19" r:id="rId9" display="Password@123" xr:uid="{D05C35DE-D138-4810-B1AC-59CDB7E5213C}"/>
+    <hyperlink ref="G20" r:id="rId10" display="Password@123" xr:uid="{8C9443A3-AC63-4830-AA68-FED07FD75DF1}"/>
     <hyperlink ref="B11" r:id="rId11" xr:uid="{591476FC-7F4D-4E21-95FB-FE905F06224D}"/>
     <hyperlink ref="B12" r:id="rId12" xr:uid="{E08AF20F-1925-48B2-ADC6-E871D2310CB2}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{BAC96627-CAAB-4E68-B565-D169A2F01E27}"/>
+    <hyperlink ref="F21" r:id="rId14" display="Password@123" xr:uid="{318CA6CF-9D7E-47AF-A827-A163222374BA}"/>
+    <hyperlink ref="G21" r:id="rId15" display="Password@123" xr:uid="{676F62B9-E808-49F7-9690-72DE17DFB513}"/>
+    <hyperlink ref="F28" r:id="rId16" display="Password@123" xr:uid="{AD9AB25E-100E-4D8B-B621-EDA249319974}"/>
+    <hyperlink ref="F29" r:id="rId17" display="Password@123" xr:uid="{AF7BE5C4-58B2-4BC3-BD6A-AD0FD281C7FC}"/>
+    <hyperlink ref="F30" r:id="rId18" display="Password@123" xr:uid="{9E2331DA-06FA-48FE-8B7E-337BEE8D29D4}"/>
+    <hyperlink ref="G28" r:id="rId19" display="Password@123" xr:uid="{8D78D74F-630F-4A03-A70E-9833399C8CC0}"/>
+    <hyperlink ref="G29" r:id="rId20" display="Password@123" xr:uid="{7103B670-5C0E-445E-AF9D-7FF64BA9C03F}"/>
+    <hyperlink ref="G30" r:id="rId21" display="Password@123" xr:uid="{4BA494C7-35C2-4DF2-BCEC-C4DB78827332}"/>
+    <hyperlink ref="F31" r:id="rId22" display="Password@123" xr:uid="{E4AD827C-FC0B-4ED7-9911-387BF9742319}"/>
+    <hyperlink ref="G31" r:id="rId23" display="Password@123" xr:uid="{1F091D6A-73A8-424A-9D8C-04C50B98B882}"/>
+    <hyperlink ref="E31" r:id="rId24" xr:uid="{26FF543D-4E26-4E28-A3E6-C3CE7ED34923}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>